<commit_message>
[DONE] Fix upload failed on CreateExercise.js (#65)
* Fix attachment and playback times in Create Exercise

* Update Sample-Exercise.xlsx

* Fix attachment and playback times in Create Exam

* Update Sample-Exam.xlsx

* modify exercise parser

* add error handler

Co-authored-by: Ramandika Pranamulia <theone_rama@yahoo.com>
</commit_message>
<xml_diff>
--- a/public/excel/Sample-Exam.xlsx
+++ b/public/excel/Sample-Exam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalahudin Al Ayyub\Documents\Klassiq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web_development\edufrontend\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D39B88-2EDA-4A90-AB18-50A3E51D8AD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0664340F-26BF-4363-BA59-52C5A7A7C018}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9264F1A3-570B-41A4-8AE8-AB0DB4E1452B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9264F1A3-570B-41A4-8AE8-AB0DB4E1452B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,12 +72,6 @@
     <t>Wrong Score</t>
   </si>
   <si>
-    <t>Listen to the conversation. Where did Agus get back from?</t>
-  </si>
-  <si>
-    <t>https://mcdn.podbean.com/mf/web/24psp6/2_Navigating_the_path_to_fluency64292.mp3</t>
-  </si>
-  <si>
     <t>Market</t>
   </si>
   <si>
@@ -87,15 +81,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Ujian Akhir Semester 2020/2021</t>
-  </si>
-  <si>
     <t>Ini bisa diisi materi yang terkait dengan ujian</t>
   </si>
   <si>
-    <t>Listen to the conversation. Where did Budi get back from?</t>
-  </si>
-  <si>
     <t>Joni</t>
   </si>
   <si>
@@ -121,6 +109,18 @@
   </si>
   <si>
     <t>22/02/2021 12.40</t>
+  </si>
+  <si>
+    <t>Listen to the conversation. Where did Agus get back from?QWER</t>
+  </si>
+  <si>
+    <t>Listen to the conversation. Where did Budi get back from?QWER</t>
+  </si>
+  <si>
+    <t>["https://mcdn.podbean.com/mf/web/24psp6/2_Navigating_the_path_to_fluency64292.mp3"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ujian Akhir Semester 2020/2021 </t>
   </si>
 </sst>
 </file>
@@ -541,7 +541,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -571,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="4" spans="2:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1">
         <v>30</v>
@@ -599,7 +599,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -613,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -624,10 +624,10 @@
     </row>
     <row r="7" spans="2:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -662,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -670,19 +670,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -699,19 +699,19 @@
         <v>2</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H10" s="2">
         <v>5</v>
@@ -720,7 +720,7 @@
         <v>-3</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -756,8 +756,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{76D931F8-CC89-4C8E-8985-4F02DD49E21F}"/>
-    <hyperlink ref="D10" r:id="rId2" xr:uid="{24E8D402-8202-4135-81A9-0504500410EE}"/>
+    <hyperlink ref="D9" r:id="rId1" display="https://mcdn.podbean.com/mf/web/24psp6/2_Navigating_the_path_to_fluency64292.mp3" xr:uid="{76D931F8-CC89-4C8E-8985-4F02DD49E21F}"/>
+    <hyperlink ref="D10" r:id="rId2" display="https://mcdn.podbean.com/mf/web/24psp6/2_Navigating_the_path_to_fluency64292.mp3" xr:uid="{24E8D402-8202-4135-81A9-0504500410EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>